<commit_message>
10/17/24 commit - update overall standing
</commit_message>
<xml_diff>
--- a/public/results/Overall Standings.xlsx
+++ b/public/results/Overall Standings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\CODE\golf-league-site\public\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8BB98E9-A808-4A6E-B087-A2A132E89603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96A1D35-B540-4DC5-BB1E-3D2E4F7AB14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1470" windowWidth="22305" windowHeight="13695" xr2:uid="{CA13D0E1-B198-4A8F-AFA4-574A5497A311}"/>
+    <workbookView xWindow="1680" yWindow="1395" windowWidth="22305" windowHeight="13695" xr2:uid="{CA13D0E1-B198-4A8F-AFA4-574A5497A311}"/>
   </bookViews>
   <sheets>
     <sheet name="2024 Overall" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>As of Week 22  (9/30/24)</t>
   </si>
@@ -153,13 +153,34 @@
   </si>
   <si>
     <t>= Under min # of rounds</t>
+  </si>
+  <si>
+    <t>Mark Young</t>
+  </si>
+  <si>
+    <t>Mark Hutter</t>
+  </si>
+  <si>
+    <t>John Bess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Champion: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second: </t>
+  </si>
+  <si>
+    <t>Overall Winners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +203,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -197,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -236,32 +265,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -492,70 +495,80 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -564,60 +577,80 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,668 +985,699 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A067D08-1B74-466D-AE0E-601BAA7BD003}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="5"/>
-    <col min="7" max="7" width="3.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="41" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="41" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="42" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="7.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="3.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="34" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" style="34" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="35" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="38" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="34" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="H1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="48"/>
+      <c r="J1" s="49"/>
+      <c r="L1" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="44"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="H2" s="11" t="s">
+      <c r="F2" s="5"/>
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="5"/>
+      <c r="L2" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="L3" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="15">
         <v>206</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="16">
         <v>11</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="15">
         <v>117</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="16">
         <v>6</v>
       </c>
-      <c r="H4" s="24">
-        <f>C4+E4</f>
+      <c r="H4" s="17">
+        <f t="shared" ref="H4:H21" si="0">C4+E4</f>
         <v>323</v>
       </c>
-      <c r="I4" s="25">
-        <f>D4+F4</f>
+      <c r="I4" s="18">
+        <f t="shared" ref="I4:I21" si="1">D4+F4</f>
         <v>17</v>
       </c>
-      <c r="J4" s="26">
-        <f>H4/I4</f>
+      <c r="J4" s="19">
+        <f t="shared" ref="J4:J21" si="2">H4/I4</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="L4" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="20">
         <v>126</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="21">
         <v>7</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="22">
         <v>176</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="21">
         <v>9</v>
       </c>
-      <c r="H5" s="30">
-        <f>C5+E5</f>
+      <c r="H5" s="23">
+        <f t="shared" si="0"/>
         <v>302</v>
       </c>
-      <c r="I5" s="31">
-        <f>D5+F5</f>
+      <c r="I5" s="24">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J5" s="32">
-        <f>H5/I5</f>
+      <c r="J5" s="25">
+        <f t="shared" si="2"/>
         <v>18.875</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="20">
         <v>166</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="21">
         <v>9</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="22">
         <v>116</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="21">
         <v>6</v>
       </c>
-      <c r="H6" s="30">
-        <f>C6+E6</f>
+      <c r="H6" s="23">
+        <f t="shared" si="0"/>
         <v>282</v>
       </c>
-      <c r="I6" s="31">
-        <f>D6+F6</f>
+      <c r="I6" s="24">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J6" s="32">
-        <f>H6/I6</f>
+      <c r="J6" s="25">
+        <f t="shared" si="2"/>
         <v>18.8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="20">
         <v>127</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="21">
         <v>7</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="22">
         <v>154</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="21">
         <v>8</v>
       </c>
-      <c r="H7" s="30">
-        <f>C7+E7</f>
+      <c r="H7" s="23">
+        <f t="shared" si="0"/>
         <v>281</v>
       </c>
-      <c r="I7" s="31">
-        <f>D7+F7</f>
+      <c r="I7" s="24">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J7" s="32">
-        <f>H7/I7</f>
+      <c r="J7" s="25">
+        <f t="shared" si="2"/>
         <v>18.733333333333334</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="20">
         <v>115</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="21">
         <v>6</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="22">
         <v>127</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="21">
         <v>7</v>
       </c>
-      <c r="H8" s="30">
-        <f>C8+E8</f>
+      <c r="H8" s="23">
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
-      <c r="I8" s="31">
-        <f>D8+F8</f>
+      <c r="I8" s="24">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J8" s="32">
-        <f>H8/I8</f>
+      <c r="J8" s="25">
+        <f t="shared" si="2"/>
         <v>18.615384615384617</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="20">
         <v>189</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="21">
         <v>10</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="22">
         <v>139</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="21">
         <v>8</v>
       </c>
-      <c r="H9" s="30">
-        <f>C9+E9</f>
+      <c r="H9" s="23">
+        <f t="shared" si="0"/>
         <v>328</v>
       </c>
-      <c r="I9" s="31">
-        <f>D9+F9</f>
+      <c r="I9" s="24">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="J9" s="32">
-        <f>H9/I9</f>
+      <c r="J9" s="25">
+        <f t="shared" si="2"/>
         <v>18.222222222222221</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="20">
         <v>127</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="21">
         <v>7</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="22">
         <v>127</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="21">
         <v>7</v>
       </c>
-      <c r="H10" s="30">
-        <f>C10+E10</f>
+      <c r="H10" s="23">
+        <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="I10" s="31">
-        <f>D10+F10</f>
+      <c r="I10" s="24">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J10" s="32">
-        <f>H10/I10</f>
+      <c r="J10" s="25">
+        <f t="shared" si="2"/>
         <v>18.142857142857142</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="20">
         <v>166</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="21">
         <v>9</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="22">
         <v>114</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="21">
         <v>7</v>
       </c>
-      <c r="H11" s="30">
-        <f>C11+E11</f>
+      <c r="H11" s="23">
+        <f t="shared" si="0"/>
         <v>280</v>
       </c>
-      <c r="I11" s="31">
-        <f>D11+F11</f>
+      <c r="I11" s="24">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J11" s="32">
-        <f>H11/I11</f>
+      <c r="J11" s="25">
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="20">
         <v>146</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="21">
         <v>8</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="22">
         <v>81</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="26">
         <v>5</v>
       </c>
-      <c r="H12" s="30">
-        <f>C12+E12</f>
+      <c r="H12" s="23">
+        <f t="shared" si="0"/>
         <v>227</v>
       </c>
-      <c r="I12" s="31">
-        <f>D12+F12</f>
+      <c r="I12" s="24">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J12" s="32">
-        <f>H12/I12</f>
+      <c r="J12" s="25">
+        <f t="shared" si="2"/>
         <v>17.46153846153846</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="27">
-        <v>0</v>
-      </c>
-      <c r="D13" s="33">
-        <v>0</v>
-      </c>
-      <c r="E13" s="29">
+      <c r="C13" s="20">
+        <v>0</v>
+      </c>
+      <c r="D13" s="26">
+        <v>0</v>
+      </c>
+      <c r="E13" s="22">
         <v>119</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="21">
         <v>6</v>
       </c>
-      <c r="H13" s="30">
-        <f>C13+E13</f>
+      <c r="H13" s="23">
+        <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="I13" s="34">
-        <f>D13+F13</f>
+      <c r="I13" s="27">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J13" s="32">
-        <f>H13/I13</f>
+      <c r="J13" s="25">
+        <f t="shared" si="2"/>
         <v>19.833333333333332</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="20">
         <v>169</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="21">
         <v>9</v>
       </c>
-      <c r="E14" s="29">
-        <v>0</v>
-      </c>
-      <c r="F14" s="33">
-        <v>0</v>
-      </c>
-      <c r="H14" s="30">
-        <f>C14+E14</f>
+      <c r="E14" s="22">
+        <v>0</v>
+      </c>
+      <c r="F14" s="26">
+        <v>0</v>
+      </c>
+      <c r="H14" s="23">
+        <f t="shared" si="0"/>
         <v>169</v>
       </c>
-      <c r="I14" s="34">
-        <f>D14+F14</f>
+      <c r="I14" s="27">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J14" s="32">
-        <f>H14/I14</f>
+      <c r="J14" s="25">
+        <f t="shared" si="2"/>
         <v>18.777777777777779</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="20">
         <v>88</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="26">
         <v>5</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="22">
         <v>93</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="26">
         <v>5</v>
       </c>
-      <c r="H15" s="30">
-        <f>C15+E15</f>
+      <c r="H15" s="23">
+        <f t="shared" si="0"/>
         <v>181</v>
       </c>
-      <c r="I15" s="34">
-        <f>D15+F15</f>
+      <c r="I15" s="27">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J15" s="32">
-        <f>H15/I15</f>
+      <c r="J15" s="25">
+        <f t="shared" si="2"/>
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="20">
         <v>72</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="26">
         <v>4</v>
       </c>
-      <c r="E16" s="29">
-        <v>0</v>
-      </c>
-      <c r="F16" s="33">
-        <v>0</v>
-      </c>
-      <c r="H16" s="30">
-        <f>C16+E16</f>
+      <c r="E16" s="22">
+        <v>0</v>
+      </c>
+      <c r="F16" s="26">
+        <v>0</v>
+      </c>
+      <c r="H16" s="23">
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="I16" s="34">
-        <f>D16+F16</f>
+      <c r="I16" s="27">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J16" s="32">
-        <f>H16/I16</f>
+      <c r="J16" s="25">
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="20">
         <v>102</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="21">
         <v>6</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="22">
         <v>71</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="26">
         <v>4</v>
       </c>
-      <c r="H17" s="30">
-        <f>C17+E17</f>
+      <c r="H17" s="23">
+        <f t="shared" si="0"/>
         <v>173</v>
       </c>
-      <c r="I17" s="34">
-        <f>D17+F17</f>
+      <c r="I17" s="27">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J17" s="32">
-        <f>H17/I17</f>
+      <c r="J17" s="25">
+        <f t="shared" si="2"/>
         <v>17.3</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="27">
-        <v>0</v>
-      </c>
-      <c r="D18" s="33">
+      <c r="C18" s="20">
+        <v>0</v>
+      </c>
+      <c r="D18" s="26">
         <v>1</v>
       </c>
-      <c r="E18" s="29">
-        <v>0</v>
-      </c>
-      <c r="F18" s="33">
+      <c r="E18" s="22">
+        <v>0</v>
+      </c>
+      <c r="F18" s="26">
         <v>1</v>
       </c>
-      <c r="H18" s="30">
-        <f>C18+E18</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="34">
-        <f>D18+F18</f>
+      <c r="H18" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="27">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J18" s="35">
-        <f>H18/I18</f>
+      <c r="J18" s="28">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="27">
-        <v>0</v>
-      </c>
-      <c r="D19" s="33">
+      <c r="C19" s="20">
+        <v>0</v>
+      </c>
+      <c r="D19" s="26">
         <v>1</v>
       </c>
-      <c r="E19" s="29">
-        <v>0</v>
-      </c>
-      <c r="F19" s="33">
-        <v>0</v>
-      </c>
-      <c r="H19" s="30">
-        <f>C19+E19</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="34">
-        <f>D19+F19</f>
+      <c r="E19" s="22">
+        <v>0</v>
+      </c>
+      <c r="F19" s="26">
+        <v>0</v>
+      </c>
+      <c r="H19" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="27">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J19" s="35">
-        <f>H19/I19</f>
+      <c r="J19" s="28">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="27">
-        <v>0</v>
-      </c>
-      <c r="D20" s="33">
-        <v>0</v>
-      </c>
-      <c r="E20" s="29">
-        <v>0</v>
-      </c>
-      <c r="F20" s="33">
+      <c r="C20" s="20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="26">
+        <v>0</v>
+      </c>
+      <c r="E20" s="22">
+        <v>0</v>
+      </c>
+      <c r="F20" s="26">
         <v>1</v>
       </c>
-      <c r="H20" s="30">
-        <f>C20+E20</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="34">
-        <f>D20+F20</f>
+      <c r="H20" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="27">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J20" s="35">
-        <f>H20/I20</f>
+      <c r="J20" s="28">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="36">
-        <v>0</v>
-      </c>
-      <c r="D21" s="37">
+      <c r="C21" s="29">
+        <v>0</v>
+      </c>
+      <c r="D21" s="30">
         <v>1</v>
       </c>
-      <c r="E21" s="38">
-        <v>0</v>
-      </c>
-      <c r="F21" s="37">
-        <v>0</v>
-      </c>
-      <c r="H21" s="39">
-        <f>C21+E21</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="40">
-        <f>D21+F21</f>
+      <c r="E21" s="31">
+        <v>0</v>
+      </c>
+      <c r="F21" s="30">
+        <v>0</v>
+      </c>
+      <c r="H21" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="33">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J21" s="19">
-        <f>H21/I21</f>
+      <c r="J21" s="12">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="43"/>
-      <c r="D23" s="44" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
10/17/24 commit - added CTTP winner
</commit_message>
<xml_diff>
--- a/public/results/Overall Standings.xlsx
+++ b/public/results/Overall Standings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\CODE\golf-league-site\public\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96A1D35-B540-4DC5-BB1E-3D2E4F7AB14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892E46E0-6AC4-4675-B8C6-7BD6001093EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="1395" windowWidth="22305" windowHeight="13695" xr2:uid="{CA13D0E1-B198-4A8F-AFA4-574A5497A311}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>As of Week 22  (9/30/24)</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t xml:space="preserve">Third: </t>
+  </si>
+  <si>
+    <t>Jon Dickey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closest to the Pin: </t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -510,11 +516,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -628,29 +660,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,7 +1025,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1041,7 @@
     <col min="9" max="9" width="8.42578125" style="34" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" style="35" customWidth="1"/>
     <col min="11" max="11" width="4.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="38" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="38" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" style="34" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1012,20 +1049,19 @@
     <row r="1" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24"/>
       <c r="B1" s="24"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="49"/>
-      <c r="L1" s="43" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45"/>
+      <c r="H1" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="49"/>
+      <c r="J1" s="50"/>
+      <c r="L1" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="44"/>
+      <c r="M1" s="47"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -1046,7 +1082,7 @@
       <c r="L2" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="43" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1081,7 +1117,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
@@ -1112,14 +1148,14 @@
         <f t="shared" ref="J4:J21" si="2">H4/I4</f>
         <v>19</v>
       </c>
-      <c r="L4" s="42" t="s">
+      <c r="L4" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="52" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1149,6 +1185,12 @@
       <c r="J5" s="25">
         <f t="shared" si="2"/>
         <v>18.875</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>